<commit_message>
created mazes and 8x8 grids
</commit_message>
<xml_diff>
--- a/search_results.xlsx
+++ b/search_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t># blocks</t>
   </si>
@@ -43,7 +43,19 @@
     <t>unidirectional t-s</t>
   </si>
   <si>
+    <t>bidirectional</t>
+  </si>
+  <si>
     <t>[N/A,N/A]</t>
+  </si>
+  <si>
+    <t>[39,45]</t>
+  </si>
+  <si>
+    <t>[50,44]</t>
+  </si>
+  <si>
+    <t>[48,56]</t>
   </si>
   <si>
     <t>file_path_here</t>
@@ -404,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,19 +453,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>280</v>
+        <v>1147</v>
       </c>
       <c r="D2">
-        <v>91</v>
+        <v>2455</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -464,19 +476,180 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>280</v>
+        <v>635</v>
       </c>
       <c r="D3">
-        <v>83</v>
+        <v>1233</v>
       </c>
       <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+      <c r="D4">
+        <v>2595</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>57386</v>
+      </c>
+      <c r="D5">
+        <v>141570</v>
+      </c>
+      <c r="E5">
+        <v>168</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>12553</v>
+      </c>
+      <c r="D6">
+        <v>29873</v>
+      </c>
+      <c r="E6">
+        <v>127</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C7">
+        <v>42732</v>
+      </c>
+      <c r="D7">
+        <v>123682</v>
+      </c>
+      <c r="E7">
+        <v>160</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>160153</v>
+      </c>
+      <c r="D8">
+        <v>558700</v>
+      </c>
+      <c r="E8">
+        <v>164</v>
+      </c>
+      <c r="F8" t="s">
         <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3210905</v>
+      </c>
+      <c r="D9">
+        <v>9188381</v>
+      </c>
+      <c r="E9">
+        <v>164</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1626921</v>
+      </c>
+      <c r="D10">
+        <v>38987985</v>
+      </c>
+      <c r="E10">
+        <v>169</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed main to 4d cube
</commit_message>
<xml_diff>
--- a/search_results.xlsx
+++ b/search_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t># blocks</t>
   </si>
@@ -37,19 +37,10 @@
     <t>Grid with Solution</t>
   </si>
   <si>
-    <t>unidirectional s-t</t>
-  </si>
-  <si>
-    <t>unidirectional t-s</t>
-  </si>
-  <si>
     <t>bidirectional</t>
   </si>
   <si>
-    <t>[N/A,N/A]</t>
-  </si>
-  <si>
-    <t>[6,7]</t>
+    <t>[7,0]</t>
   </si>
   <si>
     <t>file_path_here</t>
@@ -410,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,65 +438,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>35989</v>
+        <v>525</v>
       </c>
       <c r="D2">
-        <v>23151</v>
+        <v>200</v>
       </c>
       <c r="E2">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>35989</v>
-      </c>
-      <c r="D3">
-        <v>27685</v>
-      </c>
-      <c r="E3">
-        <v>109</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4">
-        <v>5715</v>
-      </c>
-      <c r="D4">
-        <v>9323</v>
-      </c>
-      <c r="E4">
-        <v>99</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests on SM grids
</commit_message>
<xml_diff>
--- a/search_results.xlsx
+++ b/search_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="14">
   <si>
     <t># blocks</t>
   </si>
@@ -37,10 +37,22 @@
     <t>Grid with Solution</t>
   </si>
   <si>
+    <t>unidirectional s-t</t>
+  </si>
+  <si>
+    <t>unidirectional t-s</t>
+  </si>
+  <si>
     <t>bidirectional</t>
   </si>
   <si>
-    <t>[9,4]</t>
+    <t>[N/A,N/A]</t>
+  </si>
+  <si>
+    <t>[10,12]</t>
+  </si>
+  <si>
+    <t>[11,11]</t>
   </si>
   <si>
     <t>file_path_here</t>
@@ -401,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,25 +444,692 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>480</v>
+      </c>
+      <c r="D2">
+        <v>354</v>
+      </c>
+      <c r="E2">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>523</v>
+      </c>
+      <c r="D3">
+        <v>368</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>182</v>
+      </c>
+      <c r="D4">
+        <v>168</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>281</v>
+      </c>
+      <c r="D5">
+        <v>228</v>
+      </c>
+      <c r="E5">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>87</v>
+      </c>
+      <c r="D6">
+        <v>93</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <v>143</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>94</v>
+      </c>
+      <c r="D8">
+        <v>56</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>333</v>
+      </c>
+      <c r="D9">
+        <v>194</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>159</v>
+      </c>
+      <c r="D10">
+        <v>145</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>483</v>
+      </c>
+      <c r="D11">
+        <v>306</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>298</v>
+      </c>
+      <c r="D12">
+        <v>213</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>169</v>
+      </c>
+      <c r="D13">
+        <v>135</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>480</v>
+      </c>
+      <c r="D14">
+        <v>331</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>523</v>
+      </c>
+      <c r="D15">
+        <v>371</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>182</v>
+      </c>
+      <c r="D16">
+        <v>167</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>453</v>
-      </c>
-      <c r="D2">
-        <v>735</v>
-      </c>
-      <c r="E2">
-        <v>355</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>332</v>
+      </c>
+      <c r="D17">
+        <v>226</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>466</v>
+      </c>
+      <c r="D18">
+        <v>289</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>167</v>
+      </c>
+      <c r="D19">
+        <v>163</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>482</v>
+      </c>
+      <c r="D20">
+        <v>342</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>523</v>
+      </c>
+      <c r="D21">
+        <v>387</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>184</v>
+      </c>
+      <c r="D22">
+        <v>175</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>310</v>
+      </c>
+      <c r="D23">
+        <v>211</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>298</v>
+      </c>
+      <c r="D24">
+        <v>186</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>244</v>
+      </c>
+      <c r="D25">
+        <v>202</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>480</v>
+      </c>
+      <c r="D26">
+        <v>336</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>523</v>
+      </c>
+      <c r="D27">
+        <v>363</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>182</v>
+      </c>
+      <c r="D28">
+        <v>155</v>
+      </c>
+      <c r="E28">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>479</v>
+      </c>
+      <c r="D29">
+        <v>279</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>514</v>
+      </c>
+      <c r="D30">
+        <v>271</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>227</v>
+      </c>
+      <c r="D31">
+        <v>195</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better graphs (s-t connected always)
</commit_message>
<xml_diff>
--- a/search_results.xlsx
+++ b/search_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="17">
   <si>
     <t># blocks</t>
   </si>
@@ -49,10 +49,19 @@
     <t>[N/A,N/A]</t>
   </si>
   <si>
-    <t>[10,12]</t>
-  </si>
-  <si>
-    <t>[11,11]</t>
+    <t>[9,7]</t>
+  </si>
+  <si>
+    <t>[10,10]</t>
+  </si>
+  <si>
+    <t>[9,9]</t>
+  </si>
+  <si>
+    <t>[7,9]</t>
+  </si>
+  <si>
+    <t>[8,8]</t>
   </si>
   <si>
     <t>file_path_here</t>
@@ -450,19 +459,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>480</v>
+        <v>41</v>
       </c>
       <c r="D2">
-        <v>354</v>
+        <v>122</v>
       </c>
       <c r="E2">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -473,19 +482,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>523</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>368</v>
+        <v>86</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>137</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -496,19 +505,19 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>182</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -519,19 +528,19 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>281</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>228</v>
+        <v>94</v>
       </c>
       <c r="E5">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -542,19 +551,19 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>203</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -565,19 +574,19 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>150</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -588,19 +597,19 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>140</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -611,19 +620,19 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>333</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>194</v>
+        <v>137</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -634,19 +643,19 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="D10">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -657,19 +666,19 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>483</v>
+        <v>26</v>
       </c>
       <c r="D11">
-        <v>306</v>
+        <v>107</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -680,19 +689,19 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>298</v>
+        <v>31</v>
       </c>
       <c r="D12">
-        <v>213</v>
+        <v>86</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -703,19 +712,19 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -726,19 +735,19 @@
         <v>7</v>
       </c>
       <c r="C14">
-        <v>480</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>331</v>
+        <v>78</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -749,19 +758,19 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>523</v>
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>371</v>
+        <v>70</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -772,19 +781,19 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>182</v>
+        <v>18</v>
       </c>
       <c r="D16">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -795,19 +804,19 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>332</v>
+        <v>70</v>
       </c>
       <c r="D17">
-        <v>226</v>
+        <v>304</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -818,19 +827,19 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>466</v>
+        <v>70</v>
       </c>
       <c r="D18">
-        <v>289</v>
+        <v>322</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>271</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -841,19 +850,19 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>167</v>
+        <v>51</v>
       </c>
       <c r="D19">
-        <v>163</v>
+        <v>476</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -864,19 +873,19 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <v>482</v>
+        <v>41</v>
       </c>
       <c r="D20">
-        <v>342</v>
+        <v>155</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -887,19 +896,19 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>523</v>
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>387</v>
+        <v>146</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -910,19 +919,19 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>184</v>
+        <v>28</v>
       </c>
       <c r="D22">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="E22">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -933,19 +942,19 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>310</v>
+        <v>49</v>
       </c>
       <c r="D23">
-        <v>211</v>
+        <v>245</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -956,19 +965,19 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>298</v>
+        <v>150</v>
       </c>
       <c r="D24">
-        <v>186</v>
+        <v>476</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -979,19 +988,19 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>244</v>
+        <v>43</v>
       </c>
       <c r="D25">
-        <v>202</v>
+        <v>290</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1002,19 +1011,19 @@
         <v>7</v>
       </c>
       <c r="C26">
-        <v>480</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>336</v>
+        <v>26</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1025,19 +1034,19 @@
         <v>8</v>
       </c>
       <c r="C27">
-        <v>523</v>
+        <v>22</v>
       </c>
       <c r="D27">
-        <v>363</v>
+        <v>62</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1048,19 +1057,19 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="D28">
-        <v>155</v>
+        <v>58</v>
       </c>
       <c r="E28">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1071,19 +1080,19 @@
         <v>7</v>
       </c>
       <c r="C29">
-        <v>479</v>
+        <v>49</v>
       </c>
       <c r="D29">
-        <v>279</v>
+        <v>213</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>221</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1094,19 +1103,19 @@
         <v>8</v>
       </c>
       <c r="C30">
-        <v>514</v>
+        <v>29</v>
       </c>
       <c r="D30">
-        <v>271</v>
+        <v>86</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1117,19 +1126,19 @@
         <v>9</v>
       </c>
       <c r="C31">
-        <v>227</v>
+        <v>27</v>
       </c>
       <c r="D31">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>